<commit_message>
Regenerated SML IG outputs - refined examples & added CDA IG to outputs
</commit_message>
<xml_diff>
--- a/output/SharedMedicinesList/allergyintolerance-summary-1.xlsx
+++ b/output/SharedMedicinesList/allergyintolerance-summary-1.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AL$36</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AL$37</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1217" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1251" uniqueCount="289">
   <si>
     <t>Path</t>
   </si>
@@ -334,7 +334,7 @@
     <t>DomainResource.extension</t>
   </si>
   <si>
-    <t>recorderRelatedPerson</t>
+    <t>authorRelatedPerson</t>
   </si>
   <si>
     <t xml:space="preserve">Extension {http://hl7.org.au/fhir/StructureDefinition/author-related-person}
@@ -352,7 +352,14 @@
   </si>
   <si>
     <t>ele-1:All FHIR elements must have a @value or children {hasValue() | (children().count() &gt; id.count())}
-ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}inv-dh-ait-04:A related person shall conform to Base RelatedPerson {resolve().conformsTo('http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/relatedperson-dh-base-1')}</t>
+ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}</t>
+  </si>
+  <si>
+    <t>recorderRelatedPerson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inv-dh-ait-04:A related person shall conform to Base RelatedPerson {resolve().conformsTo('http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/relatedperson-dh-base-1')}
+</t>
   </si>
   <si>
     <t>AllergyIntolerance.modifierExtension</t>
@@ -1081,7 +1088,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AL36"/>
+  <dimension ref="A1:AL37"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -2104,7 +2111,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" hidden="true">
       <c r="A10" t="s" s="2">
         <v>94</v>
       </c>
@@ -2122,7 +2129,7 @@
         <v>50</v>
       </c>
       <c r="G10" t="s" s="2">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="H10" t="s" s="2">
         <v>42</v>
@@ -2212,13 +2219,15 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" hidden="true">
+    <row r="11">
       <c r="A11" t="s" s="2">
+        <v>94</v>
+      </c>
+      <c r="B11" t="s" s="2">
         <v>107</v>
       </c>
-      <c r="B11" s="2"/>
       <c r="C11" t="s" s="2">
-        <v>108</v>
+        <v>42</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" t="s" s="2">
@@ -2228,10 +2237,10 @@
         <v>41</v>
       </c>
       <c r="G11" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="H11" t="s" s="2">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="I11" t="s" s="2">
         <v>42</v>
@@ -2240,14 +2249,12 @@
         <v>95</v>
       </c>
       <c r="K11" t="s" s="2">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="L11" t="s" s="2">
-        <v>110</v>
-      </c>
-      <c r="M11" t="s" s="2">
-        <v>111</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="M11" s="2"/>
       <c r="N11" s="2"/>
       <c r="O11" t="s" s="2">
         <v>42</v>
@@ -2296,7 +2303,7 @@
         <v>42</v>
       </c>
       <c r="AE11" t="s" s="2">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="AF11" t="s" s="2">
         <v>40</v>
@@ -2308,10 +2315,10 @@
         <v>42</v>
       </c>
       <c r="AI11" t="s" s="2">
-        <v>42</v>
+        <v>108</v>
       </c>
       <c r="AJ11" t="s" s="2">
-        <v>93</v>
+        <v>42</v>
       </c>
       <c r="AK11" t="s" s="2">
         <v>42</v>
@@ -2322,11 +2329,11 @@
     </row>
     <row r="12" hidden="true">
       <c r="A12" t="s" s="2">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s" s="2">
-        <v>42</v>
+        <v>110</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" t="s" s="2">
@@ -2339,21 +2346,23 @@
         <v>42</v>
       </c>
       <c r="H12" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="I12" t="s" s="2">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="J12" t="s" s="2">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="K12" t="s" s="2">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="L12" t="s" s="2">
-        <v>116</v>
-      </c>
-      <c r="M12" s="2"/>
+        <v>112</v>
+      </c>
+      <c r="M12" t="s" s="2">
+        <v>113</v>
+      </c>
       <c r="N12" s="2"/>
       <c r="O12" t="s" s="2">
         <v>42</v>
@@ -2402,7 +2411,7 @@
         <v>42</v>
       </c>
       <c r="AE12" t="s" s="2">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AF12" t="s" s="2">
         <v>40</v>
@@ -2417,18 +2426,18 @@
         <v>42</v>
       </c>
       <c r="AJ12" t="s" s="2">
-        <v>117</v>
+        <v>93</v>
       </c>
       <c r="AK12" t="s" s="2">
-        <v>117</v>
+        <v>42</v>
       </c>
       <c r="AL12" t="s" s="2">
-        <v>118</v>
+        <v>42</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" hidden="true">
       <c r="A13" t="s" s="2">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" t="s" s="2">
@@ -2439,29 +2448,27 @@
         <v>40</v>
       </c>
       <c r="F13" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="G13" t="s" s="2">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="H13" t="s" s="2">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="I13" t="s" s="2">
         <v>51</v>
       </c>
       <c r="J13" t="s" s="2">
-        <v>69</v>
+        <v>116</v>
       </c>
       <c r="K13" t="s" s="2">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="L13" t="s" s="2">
-        <v>121</v>
-      </c>
-      <c r="M13" t="s" s="2">
-        <v>122</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="M13" s="2"/>
       <c r="N13" s="2"/>
       <c r="O13" t="s" s="2">
         <v>42</v>
@@ -2486,13 +2493,13 @@
         <v>42</v>
       </c>
       <c r="W13" t="s" s="2">
-        <v>123</v>
+        <v>42</v>
       </c>
       <c r="X13" t="s" s="2">
-        <v>121</v>
+        <v>42</v>
       </c>
       <c r="Y13" t="s" s="2">
-        <v>124</v>
+        <v>42</v>
       </c>
       <c r="Z13" t="s" s="2">
         <v>42</v>
@@ -2510,33 +2517,33 @@
         <v>42</v>
       </c>
       <c r="AE13" t="s" s="2">
+        <v>115</v>
+      </c>
+      <c r="AF13" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG13" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AH13" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AI13" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AJ13" t="s" s="2">
         <v>119</v>
       </c>
-      <c r="AF13" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AG13" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH13" t="s" s="2">
-        <v>125</v>
-      </c>
-      <c r="AI13" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AJ13" t="s" s="2">
-        <v>126</v>
-      </c>
       <c r="AK13" t="s" s="2">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="AL13" t="s" s="2">
-        <v>42</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s" s="2">
@@ -2544,7 +2551,7 @@
       </c>
       <c r="D14" s="2"/>
       <c r="E14" t="s" s="2">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="F14" t="s" s="2">
         <v>50</v>
@@ -2562,13 +2569,13 @@
         <v>69</v>
       </c>
       <c r="K14" t="s" s="2">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="L14" t="s" s="2">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="M14" t="s" s="2">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="N14" s="2"/>
       <c r="O14" t="s" s="2">
@@ -2594,13 +2601,13 @@
         <v>42</v>
       </c>
       <c r="W14" t="s" s="2">
+        <v>125</v>
+      </c>
+      <c r="X14" t="s" s="2">
         <v>123</v>
       </c>
-      <c r="X14" t="s" s="2">
-        <v>132</v>
-      </c>
       <c r="Y14" t="s" s="2">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="Z14" t="s" s="2">
         <v>42</v>
@@ -2618,25 +2625,25 @@
         <v>42</v>
       </c>
       <c r="AE14" t="s" s="2">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="AF14" t="s" s="2">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="AG14" t="s" s="2">
         <v>50</v>
       </c>
       <c r="AH14" t="s" s="2">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="AI14" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AJ14" t="s" s="2">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="AK14" t="s" s="2">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="AL14" t="s" s="2">
         <v>42</v>
@@ -2644,15 +2651,15 @@
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s" s="2">
-        <v>136</v>
+        <v>42</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="F15" t="s" s="2">
         <v>50</v>
@@ -2661,7 +2668,7 @@
         <v>51</v>
       </c>
       <c r="H15" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="I15" t="s" s="2">
         <v>51</v>
@@ -2670,13 +2677,13 @@
         <v>69</v>
       </c>
       <c r="K15" t="s" s="2">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="L15" t="s" s="2">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="M15" t="s" s="2">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="N15" s="2"/>
       <c r="O15" t="s" s="2">
@@ -2702,13 +2709,13 @@
         <v>42</v>
       </c>
       <c r="W15" t="s" s="2">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="X15" t="s" s="2">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="Y15" t="s" s="2">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="Z15" t="s" s="2">
         <v>42</v>
@@ -2726,47 +2733,47 @@
         <v>42</v>
       </c>
       <c r="AE15" t="s" s="2">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="AF15" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="AG15" t="s" s="2">
         <v>50</v>
       </c>
       <c r="AH15" t="s" s="2">
-        <v>42</v>
+        <v>127</v>
       </c>
       <c r="AI15" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AJ15" t="s" s="2">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="AK15" t="s" s="2">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="AL15" t="s" s="2">
-        <v>144</v>
+        <v>42</v>
       </c>
     </row>
-    <row r="16" hidden="true">
+    <row r="16">
       <c r="A16" t="s" s="2">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s" s="2">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" t="s" s="2">
         <v>40</v>
       </c>
       <c r="F16" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="G16" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="H16" t="s" s="2">
         <v>42</v>
@@ -2778,13 +2785,13 @@
         <v>69</v>
       </c>
       <c r="K16" t="s" s="2">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="L16" t="s" s="2">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="M16" t="s" s="2">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="N16" s="2"/>
       <c r="O16" t="s" s="2">
@@ -2810,13 +2817,13 @@
         <v>42</v>
       </c>
       <c r="W16" t="s" s="2">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="X16" t="s" s="2">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="Y16" t="s" s="2">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="Z16" t="s" s="2">
         <v>42</v>
@@ -2834,44 +2841,44 @@
         <v>42</v>
       </c>
       <c r="AE16" t="s" s="2">
+        <v>137</v>
+      </c>
+      <c r="AF16" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG16" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH16" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AI16" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AJ16" t="s" s="2">
+        <v>144</v>
+      </c>
+      <c r="AK16" t="s" s="2">
         <v>145</v>
       </c>
-      <c r="AF16" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AG16" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AH16" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AI16" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AJ16" t="s" s="2">
-        <v>152</v>
-      </c>
-      <c r="AK16" t="s" s="2">
-        <v>143</v>
-      </c>
       <c r="AL16" t="s" s="2">
-        <v>153</v>
+        <v>146</v>
       </c>
     </row>
     <row r="17" hidden="true">
       <c r="A17" t="s" s="2">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s" s="2">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" t="s" s="2">
         <v>40</v>
       </c>
       <c r="F17" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="G17" t="s" s="2">
         <v>42</v>
@@ -2886,13 +2893,13 @@
         <v>69</v>
       </c>
       <c r="K17" t="s" s="2">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="L17" t="s" s="2">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="M17" t="s" s="2">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="N17" s="2"/>
       <c r="O17" t="s" s="2">
@@ -2918,13 +2925,13 @@
         <v>42</v>
       </c>
       <c r="W17" t="s" s="2">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="X17" t="s" s="2">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="Y17" t="s" s="2">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="Z17" t="s" s="2">
         <v>42</v>
@@ -2942,47 +2949,47 @@
         <v>42</v>
       </c>
       <c r="AE17" t="s" s="2">
+        <v>147</v>
+      </c>
+      <c r="AF17" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG17" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AH17" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AI17" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AJ17" t="s" s="2">
         <v>154</v>
       </c>
-      <c r="AF17" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AG17" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH17" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AI17" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AJ17" t="s" s="2">
-        <v>161</v>
-      </c>
       <c r="AK17" t="s" s="2">
-        <v>162</v>
+        <v>145</v>
       </c>
       <c r="AL17" t="s" s="2">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" t="s" s="2">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="F18" t="s" s="2">
         <v>50</v>
       </c>
       <c r="G18" t="s" s="2">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="H18" t="s" s="2">
         <v>42</v>
@@ -2991,16 +2998,16 @@
         <v>51</v>
       </c>
       <c r="J18" t="s" s="2">
-        <v>166</v>
+        <v>69</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="M18" t="s" s="2">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="N18" s="2"/>
       <c r="O18" t="s" s="2">
@@ -3026,13 +3033,13 @@
         <v>42</v>
       </c>
       <c r="W18" t="s" s="2">
-        <v>170</v>
+        <v>125</v>
       </c>
       <c r="X18" t="s" s="2">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="Y18" t="s" s="2">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="Z18" t="s" s="2">
         <v>42</v>
@@ -3050,7 +3057,7 @@
         <v>42</v>
       </c>
       <c r="AE18" t="s" s="2">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="AF18" t="s" s="2">
         <v>40</v>
@@ -3065,22 +3072,22 @@
         <v>42</v>
       </c>
       <c r="AJ18" t="s" s="2">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="AK18" t="s" s="2">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="AL18" t="s" s="2">
-        <v>175</v>
+        <v>165</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" t="s" s="2">
@@ -3099,15 +3106,17 @@
         <v>51</v>
       </c>
       <c r="J19" t="s" s="2">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>180</v>
-      </c>
-      <c r="M19" s="2"/>
+        <v>170</v>
+      </c>
+      <c r="M19" t="s" s="2">
+        <v>171</v>
+      </c>
       <c r="N19" s="2"/>
       <c r="O19" t="s" s="2">
         <v>42</v>
@@ -3132,13 +3141,13 @@
         <v>42</v>
       </c>
       <c r="W19" t="s" s="2">
-        <v>42</v>
+        <v>172</v>
       </c>
       <c r="X19" t="s" s="2">
-        <v>42</v>
+        <v>173</v>
       </c>
       <c r="Y19" t="s" s="2">
-        <v>42</v>
+        <v>174</v>
       </c>
       <c r="Z19" t="s" s="2">
         <v>42</v>
@@ -3156,10 +3165,10 @@
         <v>42</v>
       </c>
       <c r="AE19" t="s" s="2">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="AF19" t="s" s="2">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="AG19" t="s" s="2">
         <v>50</v>
@@ -3171,26 +3180,26 @@
         <v>42</v>
       </c>
       <c r="AJ19" t="s" s="2">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="AK19" t="s" s="2">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="AL19" t="s" s="2">
-        <v>183</v>
+        <v>177</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
-        <v>42</v>
+        <v>179</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="F20" t="s" s="2">
         <v>50</v>
@@ -3202,16 +3211,16 @@
         <v>42</v>
       </c>
       <c r="I20" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="J20" t="s" s="2">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
@@ -3262,10 +3271,10 @@
         <v>42</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="AF20" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="AG20" t="s" s="2">
         <v>50</v>
@@ -3277,18 +3286,18 @@
         <v>42</v>
       </c>
       <c r="AJ20" t="s" s="2">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="AK20" t="s" s="2">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="AL20" t="s" s="2">
-        <v>42</v>
+        <v>185</v>
       </c>
     </row>
-    <row r="21" hidden="true">
+    <row r="21">
       <c r="A21" t="s" s="2">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
@@ -3302,7 +3311,7 @@
         <v>50</v>
       </c>
       <c r="G21" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="H21" t="s" s="2">
         <v>42</v>
@@ -3311,13 +3320,13 @@
         <v>42</v>
       </c>
       <c r="J21" t="s" s="2">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
@@ -3368,7 +3377,7 @@
         <v>42</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="AF21" t="s" s="2">
         <v>40</v>
@@ -3383,22 +3392,22 @@
         <v>42</v>
       </c>
       <c r="AJ21" t="s" s="2">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="AK21" t="s" s="2">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="AL21" t="s" s="2">
-        <v>196</v>
+        <v>42</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
-        <v>198</v>
+        <v>42</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" t="s" s="2">
@@ -3408,7 +3417,7 @@
         <v>50</v>
       </c>
       <c r="G22" t="s" s="2">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="H22" t="s" s="2">
         <v>42</v>
@@ -3417,13 +3426,13 @@
         <v>42</v>
       </c>
       <c r="J22" t="s" s="2">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
@@ -3474,7 +3483,7 @@
         <v>42</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="AF22" t="s" s="2">
         <v>40</v>
@@ -3489,22 +3498,22 @@
         <v>42</v>
       </c>
       <c r="AJ22" t="s" s="2">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="AK22" t="s" s="2">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="AL22" t="s" s="2">
-        <v>42</v>
+        <v>198</v>
       </c>
     </row>
-    <row r="23" hidden="true">
+    <row r="23">
       <c r="A23" t="s" s="2">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" t="s" s="2">
@@ -3514,26 +3523,24 @@
         <v>50</v>
       </c>
       <c r="G23" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="H23" t="s" s="2">
         <v>42</v>
       </c>
       <c r="I23" t="s" s="2">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="J23" t="s" s="2">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>208</v>
-      </c>
-      <c r="M23" t="s" s="2">
-        <v>209</v>
-      </c>
+        <v>203</v>
+      </c>
+      <c r="M23" s="2"/>
       <c r="N23" s="2"/>
       <c r="O23" t="s" s="2">
         <v>42</v>
@@ -3582,7 +3589,7 @@
         <v>42</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>40</v>
@@ -3597,22 +3604,22 @@
         <v>42</v>
       </c>
       <c r="AJ23" t="s" s="2">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="AK23" t="s" s="2">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="AL23" t="s" s="2">
-        <v>212</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
-        <v>42</v>
+        <v>207</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" t="s" s="2">
@@ -3628,19 +3635,19 @@
         <v>42</v>
       </c>
       <c r="I24" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="J24" t="s" s="2">
-        <v>191</v>
+        <v>208</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="M24" t="s" s="2">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="N24" s="2"/>
       <c r="O24" t="s" s="2">
@@ -3690,7 +3697,7 @@
         <v>42</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>40</v>
@@ -3705,18 +3712,18 @@
         <v>42</v>
       </c>
       <c r="AJ24" t="s" s="2">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="AK24" t="s" s="2">
-        <v>42</v>
+        <v>213</v>
       </c>
       <c r="AL24" t="s" s="2">
-        <v>42</v>
+        <v>214</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
@@ -3727,10 +3734,10 @@
         <v>40</v>
       </c>
       <c r="F25" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="G25" t="s" s="2">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="H25" t="s" s="2">
         <v>42</v>
@@ -3739,16 +3746,16 @@
         <v>42</v>
       </c>
       <c r="J25" t="s" s="2">
-        <v>219</v>
+        <v>193</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="M25" t="s" s="2">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="N25" s="2"/>
       <c r="O25" t="s" s="2">
@@ -3798,13 +3805,13 @@
         <v>42</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG25" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="AH25" t="s" s="2">
         <v>42</v>
@@ -3813,7 +3820,7 @@
         <v>42</v>
       </c>
       <c r="AJ25" t="s" s="2">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="AK25" t="s" s="2">
         <v>42</v>
@@ -3824,7 +3831,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s" s="2">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
@@ -3847,15 +3854,17 @@
         <v>42</v>
       </c>
       <c r="J26" t="s" s="2">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>227</v>
-      </c>
-      <c r="M26" s="2"/>
+        <v>223</v>
+      </c>
+      <c r="M26" t="s" s="2">
+        <v>224</v>
+      </c>
       <c r="N26" s="2"/>
       <c r="O26" t="s" s="2">
         <v>42</v>
@@ -3904,7 +3913,7 @@
         <v>42</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="AF26" t="s" s="2">
         <v>40</v>
@@ -3916,10 +3925,10 @@
         <v>42</v>
       </c>
       <c r="AI26" t="s" s="2">
-        <v>228</v>
+        <v>42</v>
       </c>
       <c r="AJ26" t="s" s="2">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="AK26" t="s" s="2">
         <v>42</v>
@@ -3928,9 +3937,9 @@
         <v>42</v>
       </c>
     </row>
-    <row r="27" hidden="true">
+    <row r="27">
       <c r="A27" t="s" s="2">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
@@ -3941,10 +3950,10 @@
         <v>40</v>
       </c>
       <c r="F27" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="G27" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="H27" t="s" s="2">
         <v>42</v>
@@ -3953,13 +3962,13 @@
         <v>42</v>
       </c>
       <c r="J27" t="s" s="2">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
@@ -4010,22 +4019,22 @@
         <v>42</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG27" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="AH27" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AI27" t="s" s="2">
-        <v>42</v>
+        <v>230</v>
       </c>
       <c r="AJ27" t="s" s="2">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="AK27" t="s" s="2">
         <v>42</v>
@@ -4036,18 +4045,18 @@
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
-        <v>108</v>
+        <v>42</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" t="s" s="2">
         <v>40</v>
       </c>
       <c r="F28" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="G28" t="s" s="2">
         <v>42</v>
@@ -4059,17 +4068,15 @@
         <v>42</v>
       </c>
       <c r="J28" t="s" s="2">
-        <v>95</v>
+        <v>233</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>238</v>
-      </c>
-      <c r="M28" t="s" s="2">
-        <v>111</v>
-      </c>
+        <v>235</v>
+      </c>
+      <c r="M28" s="2"/>
       <c r="N28" s="2"/>
       <c r="O28" t="s" s="2">
         <v>42</v>
@@ -4118,13 +4125,13 @@
         <v>42</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG28" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="AH28" t="s" s="2">
         <v>42</v>
@@ -4133,7 +4140,7 @@
         <v>42</v>
       </c>
       <c r="AJ28" t="s" s="2">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="AK28" t="s" s="2">
         <v>42</v>
@@ -4144,11 +4151,11 @@
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
-        <v>241</v>
+        <v>110</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" t="s" s="2">
@@ -4161,22 +4168,22 @@
         <v>42</v>
       </c>
       <c r="H29" t="s" s="2">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="I29" t="s" s="2">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="J29" t="s" s="2">
         <v>95</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>109</v>
+        <v>239</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="N29" s="2"/>
       <c r="O29" t="s" s="2">
@@ -4226,7 +4233,7 @@
         <v>42</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>40</v>
@@ -4241,7 +4248,7 @@
         <v>42</v>
       </c>
       <c r="AJ29" t="s" s="2">
-        <v>93</v>
+        <v>237</v>
       </c>
       <c r="AK29" t="s" s="2">
         <v>42</v>
@@ -4250,41 +4257,41 @@
         <v>42</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
-        <v>42</v>
+        <v>243</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" t="s" s="2">
         <v>40</v>
       </c>
       <c r="F30" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="G30" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="H30" t="s" s="2">
         <v>51</v>
       </c>
-      <c r="H30" t="s" s="2">
-        <v>42</v>
-      </c>
       <c r="I30" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="J30" t="s" s="2">
-        <v>166</v>
+        <v>95</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>245</v>
+        <v>111</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>247</v>
+        <v>113</v>
       </c>
       <c r="N30" s="2"/>
       <c r="O30" t="s" s="2">
@@ -4310,13 +4317,13 @@
         <v>42</v>
       </c>
       <c r="W30" t="s" s="2">
-        <v>170</v>
+        <v>42</v>
       </c>
       <c r="X30" t="s" s="2">
-        <v>248</v>
+        <v>42</v>
       </c>
       <c r="Y30" t="s" s="2">
-        <v>249</v>
+        <v>42</v>
       </c>
       <c r="Z30" t="s" s="2">
         <v>42</v>
@@ -4334,13 +4341,13 @@
         <v>42</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG30" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="AH30" t="s" s="2">
         <v>42</v>
@@ -4349,7 +4356,7 @@
         <v>42</v>
       </c>
       <c r="AJ30" t="s" s="2">
-        <v>250</v>
+        <v>93</v>
       </c>
       <c r="AK30" t="s" s="2">
         <v>42</v>
@@ -4360,18 +4367,18 @@
     </row>
     <row r="31">
       <c r="A31" t="s" s="2">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
-        <v>252</v>
+        <v>42</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="F31" t="s" s="2">
         <v>50</v>
-      </c>
-      <c r="F31" t="s" s="2">
-        <v>41</v>
       </c>
       <c r="G31" t="s" s="2">
         <v>51</v>
@@ -4383,16 +4390,16 @@
         <v>42</v>
       </c>
       <c r="J31" t="s" s="2">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="N31" s="2"/>
       <c r="O31" t="s" s="2">
@@ -4418,13 +4425,13 @@
         <v>42</v>
       </c>
       <c r="W31" t="s" s="2">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="X31" t="s" s="2">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="Y31" t="s" s="2">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="Z31" t="s" s="2">
         <v>42</v>
@@ -4442,14 +4449,14 @@
         <v>42</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="AF31" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG31" t="s" s="2">
         <v>50</v>
       </c>
-      <c r="AG31" t="s" s="2">
-        <v>41</v>
-      </c>
       <c r="AH31" t="s" s="2">
         <v>42</v>
       </c>
@@ -4457,32 +4464,32 @@
         <v>42</v>
       </c>
       <c r="AJ31" t="s" s="2">
-        <v>142</v>
+        <v>252</v>
       </c>
       <c r="AK31" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AL31" t="s" s="2">
-        <v>258</v>
+        <v>42</v>
       </c>
     </row>
-    <row r="32" hidden="true">
+    <row r="32">
       <c r="A32" t="s" s="2">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="F32" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="G32" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="H32" t="s" s="2">
         <v>42</v>
@@ -4491,16 +4498,16 @@
         <v>42</v>
       </c>
       <c r="J32" t="s" s="2">
-        <v>231</v>
+        <v>168</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="N32" s="2"/>
       <c r="O32" t="s" s="2">
@@ -4526,13 +4533,13 @@
         <v>42</v>
       </c>
       <c r="W32" t="s" s="2">
-        <v>42</v>
+        <v>172</v>
       </c>
       <c r="X32" t="s" s="2">
-        <v>42</v>
+        <v>258</v>
       </c>
       <c r="Y32" t="s" s="2">
-        <v>42</v>
+        <v>259</v>
       </c>
       <c r="Z32" t="s" s="2">
         <v>42</v>
@@ -4550,13 +4557,13 @@
         <v>42</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="AF32" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="AG32" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="AH32" t="s" s="2">
         <v>42</v>
@@ -4565,22 +4572,22 @@
         <v>42</v>
       </c>
       <c r="AJ32" t="s" s="2">
-        <v>264</v>
+        <v>144</v>
       </c>
       <c r="AK32" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AL32" t="s" s="2">
-        <v>42</v>
+        <v>260</v>
       </c>
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
-        <v>42</v>
+        <v>262</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" t="s" s="2">
@@ -4599,15 +4606,17 @@
         <v>42</v>
       </c>
       <c r="J33" t="s" s="2">
-        <v>191</v>
+        <v>233</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>267</v>
-      </c>
-      <c r="M33" s="2"/>
+        <v>264</v>
+      </c>
+      <c r="M33" t="s" s="2">
+        <v>265</v>
+      </c>
       <c r="N33" s="2"/>
       <c r="O33" t="s" s="2">
         <v>42</v>
@@ -4656,7 +4665,7 @@
         <v>42</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>40</v>
@@ -4671,18 +4680,18 @@
         <v>42</v>
       </c>
       <c r="AJ33" t="s" s="2">
-        <v>188</v>
+        <v>266</v>
       </c>
       <c r="AK33" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AL33" t="s" s="2">
-        <v>268</v>
+        <v>42</v>
       </c>
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
@@ -4705,17 +4714,15 @@
         <v>42</v>
       </c>
       <c r="J34" t="s" s="2">
-        <v>69</v>
+        <v>193</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>271</v>
-      </c>
-      <c r="M34" t="s" s="2">
-        <v>272</v>
-      </c>
+        <v>269</v>
+      </c>
+      <c r="M34" s="2"/>
       <c r="N34" s="2"/>
       <c r="O34" t="s" s="2">
         <v>42</v>
@@ -4740,13 +4747,13 @@
         <v>42</v>
       </c>
       <c r="W34" t="s" s="2">
-        <v>123</v>
+        <v>42</v>
       </c>
       <c r="X34" t="s" s="2">
-        <v>273</v>
+        <v>42</v>
       </c>
       <c r="Y34" t="s" s="2">
-        <v>274</v>
+        <v>42</v>
       </c>
       <c r="Z34" t="s" s="2">
         <v>42</v>
@@ -4764,7 +4771,7 @@
         <v>42</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>40</v>
@@ -4779,18 +4786,18 @@
         <v>42</v>
       </c>
       <c r="AJ34" t="s" s="2">
-        <v>161</v>
+        <v>190</v>
       </c>
       <c r="AK34" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AL34" t="s" s="2">
-        <v>42</v>
+        <v>270</v>
       </c>
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -4813,16 +4820,16 @@
         <v>42</v>
       </c>
       <c r="J35" t="s" s="2">
-        <v>166</v>
+        <v>69</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="M35" t="s" s="2">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="N35" s="2"/>
       <c r="O35" t="s" s="2">
@@ -4848,13 +4855,13 @@
         <v>42</v>
       </c>
       <c r="W35" t="s" s="2">
-        <v>279</v>
+        <v>125</v>
       </c>
       <c r="X35" t="s" s="2">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="Y35" t="s" s="2">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="Z35" t="s" s="2">
         <v>42</v>
@@ -4872,7 +4879,7 @@
         <v>42</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>40</v>
@@ -4887,7 +4894,7 @@
         <v>42</v>
       </c>
       <c r="AJ35" t="s" s="2">
-        <v>282</v>
+        <v>163</v>
       </c>
       <c r="AK35" t="s" s="2">
         <v>42</v>
@@ -4898,7 +4905,7 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -4909,7 +4916,7 @@
         <v>40</v>
       </c>
       <c r="F36" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="G36" t="s" s="2">
         <v>42</v>
@@ -4921,16 +4928,16 @@
         <v>42</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>219</v>
+        <v>168</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="M36" t="s" s="2">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="N36" s="2"/>
       <c r="O36" t="s" s="2">
@@ -4956,13 +4963,13 @@
         <v>42</v>
       </c>
       <c r="W36" t="s" s="2">
-        <v>42</v>
+        <v>281</v>
       </c>
       <c r="X36" t="s" s="2">
-        <v>42</v>
+        <v>282</v>
       </c>
       <c r="Y36" t="s" s="2">
-        <v>42</v>
+        <v>283</v>
       </c>
       <c r="Z36" t="s" s="2">
         <v>42</v>
@@ -4980,32 +4987,140 @@
         <v>42</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG36" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH36" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AI36" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AJ36" t="s" s="2">
+        <v>284</v>
+      </c>
+      <c r="AK36" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AL36" t="s" s="2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="37" hidden="true">
+      <c r="A37" t="s" s="2">
+        <v>285</v>
+      </c>
+      <c r="B37" s="2"/>
+      <c r="C37" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="D37" s="2"/>
+      <c r="E37" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="F37" t="s" s="2">
         <v>41</v>
       </c>
-      <c r="AH36" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AI36" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AJ36" t="s" s="2">
-        <v>223</v>
-      </c>
-      <c r="AK36" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AL36" t="s" s="2">
+      <c r="G37" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="H37" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="I37" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="J37" t="s" s="2">
+        <v>221</v>
+      </c>
+      <c r="K37" t="s" s="2">
+        <v>286</v>
+      </c>
+      <c r="L37" t="s" s="2">
+        <v>287</v>
+      </c>
+      <c r="M37" t="s" s="2">
+        <v>288</v>
+      </c>
+      <c r="N37" s="2"/>
+      <c r="O37" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="P37" s="2"/>
+      <c r="Q37" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="R37" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="S37" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="T37" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="U37" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="V37" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="W37" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="X37" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="Y37" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="Z37" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AA37" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AB37" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AC37" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AD37" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AE37" t="s" s="2">
+        <v>285</v>
+      </c>
+      <c r="AF37" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG37" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AH37" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AI37" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AJ37" t="s" s="2">
+        <v>225</v>
+      </c>
+      <c r="AK37" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AL37" t="s" s="2">
         <v>42</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AL36">
+  <autoFilter ref="A1:AL37">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -5015,7 +5130,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI35">
+  <conditionalFormatting sqref="A2:AI36">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Regenerate SML IG outputs - new HL7 AU dependency, plus...
Updated package dependency to be http://hl7.org.au/fhir/base/aubase1.1 and revised all relevant hyperlinks throughout. 
Further revisions to mappings.md.
Fixed a bad extension in allergyintolerance-summary-1 profile.
</commit_message>
<xml_diff>
--- a/output/SharedMedicinesList/allergyintolerance-summary-1.xlsx
+++ b/output/SharedMedicinesList/allergyintolerance-summary-1.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AL$37</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AL$36</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1251" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1217" uniqueCount="287">
   <si>
     <t>Path</t>
   </si>
@@ -352,14 +352,7 @@
   </si>
   <si>
     <t>ele-1:All FHIR elements must have a @value or children {hasValue() | (children().count() &gt; id.count())}
-ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}</t>
-  </si>
-  <si>
-    <t>recorderRelatedPerson</t>
-  </si>
-  <si>
-    <t xml:space="preserve">inv-dh-ait-04:A related person shall conform to Base RelatedPerson {resolve().conformsTo('http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/relatedperson-dh-base-1')}
-</t>
+ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}inv-dh-ait-04:A related person shall conform to Base RelatedPerson {resolve().conformsTo('http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/relatedperson-dh-base-1')}</t>
   </si>
   <si>
     <t>AllergyIntolerance.modifierExtension</t>
@@ -1088,7 +1081,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AL37"/>
+  <dimension ref="A1:AL36"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -1098,7 +1091,7 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="42.24609375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="21.78125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="20.07421875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="38.81640625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="5.8984375" customWidth="true" bestFit="true" hidden="true"/>
     <col min="5" max="5" width="4.69921875" customWidth="true" bestFit="true"/>
@@ -2111,7 +2104,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" hidden="true">
+    <row r="10">
       <c r="A10" t="s" s="2">
         <v>94</v>
       </c>
@@ -2129,7 +2122,7 @@
         <v>50</v>
       </c>
       <c r="G10" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="H10" t="s" s="2">
         <v>42</v>
@@ -2219,15 +2212,13 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" hidden="true">
       <c r="A11" t="s" s="2">
-        <v>94</v>
-      </c>
-      <c r="B11" t="s" s="2">
         <v>107</v>
       </c>
+      <c r="B11" s="2"/>
       <c r="C11" t="s" s="2">
-        <v>42</v>
+        <v>108</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" t="s" s="2">
@@ -2237,10 +2228,10 @@
         <v>41</v>
       </c>
       <c r="G11" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="H11" t="s" s="2">
         <v>51</v>
-      </c>
-      <c r="H11" t="s" s="2">
-        <v>42</v>
       </c>
       <c r="I11" t="s" s="2">
         <v>42</v>
@@ -2249,12 +2240,14 @@
         <v>95</v>
       </c>
       <c r="K11" t="s" s="2">
-        <v>96</v>
+        <v>109</v>
       </c>
       <c r="L11" t="s" s="2">
-        <v>97</v>
-      </c>
-      <c r="M11" s="2"/>
+        <v>110</v>
+      </c>
+      <c r="M11" t="s" s="2">
+        <v>111</v>
+      </c>
       <c r="N11" s="2"/>
       <c r="O11" t="s" s="2">
         <v>42</v>
@@ -2303,7 +2296,7 @@
         <v>42</v>
       </c>
       <c r="AE11" t="s" s="2">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="AF11" t="s" s="2">
         <v>40</v>
@@ -2315,10 +2308,10 @@
         <v>42</v>
       </c>
       <c r="AI11" t="s" s="2">
-        <v>108</v>
+        <v>42</v>
       </c>
       <c r="AJ11" t="s" s="2">
-        <v>42</v>
+        <v>93</v>
       </c>
       <c r="AK11" t="s" s="2">
         <v>42</v>
@@ -2329,11 +2322,11 @@
     </row>
     <row r="12" hidden="true">
       <c r="A12" t="s" s="2">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s" s="2">
-        <v>110</v>
+        <v>42</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" t="s" s="2">
@@ -2346,23 +2339,21 @@
         <v>42</v>
       </c>
       <c r="H12" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="I12" t="s" s="2">
         <v>51</v>
       </c>
-      <c r="I12" t="s" s="2">
-        <v>42</v>
-      </c>
       <c r="J12" t="s" s="2">
-        <v>95</v>
+        <v>114</v>
       </c>
       <c r="K12" t="s" s="2">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="L12" t="s" s="2">
-        <v>112</v>
-      </c>
-      <c r="M12" t="s" s="2">
-        <v>113</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="M12" s="2"/>
       <c r="N12" s="2"/>
       <c r="O12" t="s" s="2">
         <v>42</v>
@@ -2411,7 +2402,7 @@
         <v>42</v>
       </c>
       <c r="AE12" t="s" s="2">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AF12" t="s" s="2">
         <v>40</v>
@@ -2426,18 +2417,18 @@
         <v>42</v>
       </c>
       <c r="AJ12" t="s" s="2">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="AK12" t="s" s="2">
-        <v>42</v>
+        <v>117</v>
       </c>
       <c r="AL12" t="s" s="2">
-        <v>42</v>
+        <v>118</v>
       </c>
     </row>
-    <row r="13" hidden="true">
+    <row r="13">
       <c r="A13" t="s" s="2">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" t="s" s="2">
@@ -2448,27 +2439,29 @@
         <v>40</v>
       </c>
       <c r="F13" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="G13" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="H13" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="I13" t="s" s="2">
         <v>51</v>
       </c>
       <c r="J13" t="s" s="2">
-        <v>116</v>
+        <v>69</v>
       </c>
       <c r="K13" t="s" s="2">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="L13" t="s" s="2">
-        <v>118</v>
-      </c>
-      <c r="M13" s="2"/>
+        <v>121</v>
+      </c>
+      <c r="M13" t="s" s="2">
+        <v>122</v>
+      </c>
       <c r="N13" s="2"/>
       <c r="O13" t="s" s="2">
         <v>42</v>
@@ -2493,13 +2486,13 @@
         <v>42</v>
       </c>
       <c r="W13" t="s" s="2">
-        <v>42</v>
+        <v>123</v>
       </c>
       <c r="X13" t="s" s="2">
-        <v>42</v>
+        <v>121</v>
       </c>
       <c r="Y13" t="s" s="2">
-        <v>42</v>
+        <v>124</v>
       </c>
       <c r="Z13" t="s" s="2">
         <v>42</v>
@@ -2517,33 +2510,33 @@
         <v>42</v>
       </c>
       <c r="AE13" t="s" s="2">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="AF13" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG13" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="AH13" t="s" s="2">
-        <v>42</v>
+        <v>125</v>
       </c>
       <c r="AI13" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AJ13" t="s" s="2">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="AK13" t="s" s="2">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="AL13" t="s" s="2">
-        <v>120</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s" s="2">
@@ -2551,7 +2544,7 @@
       </c>
       <c r="D14" s="2"/>
       <c r="E14" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="F14" t="s" s="2">
         <v>50</v>
@@ -2569,13 +2562,13 @@
         <v>69</v>
       </c>
       <c r="K14" t="s" s="2">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="L14" t="s" s="2">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="M14" t="s" s="2">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="N14" s="2"/>
       <c r="O14" t="s" s="2">
@@ -2601,49 +2594,49 @@
         <v>42</v>
       </c>
       <c r="W14" t="s" s="2">
+        <v>123</v>
+      </c>
+      <c r="X14" t="s" s="2">
+        <v>132</v>
+      </c>
+      <c r="Y14" t="s" s="2">
+        <v>133</v>
+      </c>
+      <c r="Z14" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AA14" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AB14" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AC14" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AD14" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AE14" t="s" s="2">
+        <v>128</v>
+      </c>
+      <c r="AF14" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AG14" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH14" t="s" s="2">
         <v>125</v>
       </c>
-      <c r="X14" t="s" s="2">
-        <v>123</v>
-      </c>
-      <c r="Y14" t="s" s="2">
-        <v>126</v>
-      </c>
-      <c r="Z14" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AA14" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AB14" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AC14" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AD14" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AE14" t="s" s="2">
-        <v>121</v>
-      </c>
-      <c r="AF14" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AG14" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH14" t="s" s="2">
+      <c r="AI14" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AJ14" t="s" s="2">
+        <v>134</v>
+      </c>
+      <c r="AK14" t="s" s="2">
         <v>127</v>
-      </c>
-      <c r="AI14" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AJ14" t="s" s="2">
-        <v>128</v>
-      </c>
-      <c r="AK14" t="s" s="2">
-        <v>129</v>
       </c>
       <c r="AL14" t="s" s="2">
         <v>42</v>
@@ -2651,15 +2644,15 @@
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s" s="2">
-        <v>42</v>
+        <v>136</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" t="s" s="2">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="F15" t="s" s="2">
         <v>50</v>
@@ -2668,7 +2661,7 @@
         <v>51</v>
       </c>
       <c r="H15" t="s" s="2">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="I15" t="s" s="2">
         <v>51</v>
@@ -2677,13 +2670,13 @@
         <v>69</v>
       </c>
       <c r="K15" t="s" s="2">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="L15" t="s" s="2">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="M15" t="s" s="2">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="N15" s="2"/>
       <c r="O15" t="s" s="2">
@@ -2709,71 +2702,71 @@
         <v>42</v>
       </c>
       <c r="W15" t="s" s="2">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="X15" t="s" s="2">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="Y15" t="s" s="2">
+        <v>141</v>
+      </c>
+      <c r="Z15" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AA15" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AB15" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AC15" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AD15" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AE15" t="s" s="2">
         <v>135</v>
       </c>
-      <c r="Z15" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AA15" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AB15" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AC15" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AD15" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AE15" t="s" s="2">
-        <v>130</v>
-      </c>
       <c r="AF15" t="s" s="2">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="AG15" t="s" s="2">
         <v>50</v>
       </c>
       <c r="AH15" t="s" s="2">
-        <v>127</v>
+        <v>42</v>
       </c>
       <c r="AI15" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AJ15" t="s" s="2">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="AK15" t="s" s="2">
-        <v>129</v>
+        <v>143</v>
       </c>
       <c r="AL15" t="s" s="2">
-        <v>42</v>
+        <v>144</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" hidden="true">
       <c r="A16" t="s" s="2">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s" s="2">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" t="s" s="2">
         <v>40</v>
       </c>
       <c r="F16" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="G16" t="s" s="2">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="H16" t="s" s="2">
         <v>42</v>
@@ -2785,13 +2778,13 @@
         <v>69</v>
       </c>
       <c r="K16" t="s" s="2">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="L16" t="s" s="2">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="M16" t="s" s="2">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="N16" s="2"/>
       <c r="O16" t="s" s="2">
@@ -2817,68 +2810,68 @@
         <v>42</v>
       </c>
       <c r="W16" t="s" s="2">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="X16" t="s" s="2">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="Y16" t="s" s="2">
+        <v>151</v>
+      </c>
+      <c r="Z16" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AA16" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AB16" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AC16" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AD16" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AE16" t="s" s="2">
+        <v>145</v>
+      </c>
+      <c r="AF16" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG16" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AH16" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AI16" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AJ16" t="s" s="2">
+        <v>152</v>
+      </c>
+      <c r="AK16" t="s" s="2">
         <v>143</v>
       </c>
-      <c r="Z16" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AA16" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AB16" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AC16" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AD16" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AE16" t="s" s="2">
-        <v>137</v>
-      </c>
-      <c r="AF16" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AG16" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH16" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AI16" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AJ16" t="s" s="2">
-        <v>144</v>
-      </c>
-      <c r="AK16" t="s" s="2">
-        <v>145</v>
-      </c>
       <c r="AL16" t="s" s="2">
-        <v>146</v>
+        <v>153</v>
       </c>
     </row>
     <row r="17" hidden="true">
       <c r="A17" t="s" s="2">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s" s="2">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" t="s" s="2">
         <v>40</v>
       </c>
       <c r="F17" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="G17" t="s" s="2">
         <v>42</v>
@@ -2893,13 +2886,13 @@
         <v>69</v>
       </c>
       <c r="K17" t="s" s="2">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="L17" t="s" s="2">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="M17" t="s" s="2">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="N17" s="2"/>
       <c r="O17" t="s" s="2">
@@ -2925,13 +2918,13 @@
         <v>42</v>
       </c>
       <c r="W17" t="s" s="2">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="X17" t="s" s="2">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="Y17" t="s" s="2">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="Z17" t="s" s="2">
         <v>42</v>
@@ -2949,13 +2942,13 @@
         <v>42</v>
       </c>
       <c r="AE17" t="s" s="2">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="AF17" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG17" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="AH17" t="s" s="2">
         <v>42</v>
@@ -2964,32 +2957,32 @@
         <v>42</v>
       </c>
       <c r="AJ17" t="s" s="2">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="AK17" t="s" s="2">
-        <v>145</v>
+        <v>162</v>
       </c>
       <c r="AL17" t="s" s="2">
-        <v>155</v>
+        <v>163</v>
       </c>
     </row>
-    <row r="18" hidden="true">
+    <row r="18">
       <c r="A18" t="s" s="2">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="F18" t="s" s="2">
         <v>50</v>
       </c>
       <c r="G18" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="H18" t="s" s="2">
         <v>42</v>
@@ -2998,16 +2991,16 @@
         <v>51</v>
       </c>
       <c r="J18" t="s" s="2">
-        <v>69</v>
+        <v>166</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>158</v>
+        <v>167</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>159</v>
+        <v>168</v>
       </c>
       <c r="M18" t="s" s="2">
-        <v>160</v>
+        <v>169</v>
       </c>
       <c r="N18" s="2"/>
       <c r="O18" t="s" s="2">
@@ -3033,13 +3026,13 @@
         <v>42</v>
       </c>
       <c r="W18" t="s" s="2">
-        <v>125</v>
+        <v>170</v>
       </c>
       <c r="X18" t="s" s="2">
-        <v>161</v>
+        <v>171</v>
       </c>
       <c r="Y18" t="s" s="2">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="Z18" t="s" s="2">
         <v>42</v>
@@ -3057,7 +3050,7 @@
         <v>42</v>
       </c>
       <c r="AE18" t="s" s="2">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="AF18" t="s" s="2">
         <v>40</v>
@@ -3072,22 +3065,22 @@
         <v>42</v>
       </c>
       <c r="AJ18" t="s" s="2">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="AK18" t="s" s="2">
-        <v>164</v>
+        <v>174</v>
       </c>
       <c r="AL18" t="s" s="2">
-        <v>165</v>
+        <v>175</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
-        <v>166</v>
+        <v>176</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" t="s" s="2">
@@ -3106,17 +3099,15 @@
         <v>51</v>
       </c>
       <c r="J19" t="s" s="2">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>170</v>
-      </c>
-      <c r="M19" t="s" s="2">
-        <v>171</v>
-      </c>
+        <v>180</v>
+      </c>
+      <c r="M19" s="2"/>
       <c r="N19" s="2"/>
       <c r="O19" t="s" s="2">
         <v>42</v>
@@ -3141,13 +3132,13 @@
         <v>42</v>
       </c>
       <c r="W19" t="s" s="2">
-        <v>172</v>
+        <v>42</v>
       </c>
       <c r="X19" t="s" s="2">
-        <v>173</v>
+        <v>42</v>
       </c>
       <c r="Y19" t="s" s="2">
-        <v>174</v>
+        <v>42</v>
       </c>
       <c r="Z19" t="s" s="2">
         <v>42</v>
@@ -3165,10 +3156,10 @@
         <v>42</v>
       </c>
       <c r="AE19" t="s" s="2">
-        <v>166</v>
+        <v>176</v>
       </c>
       <c r="AF19" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="AG19" t="s" s="2">
         <v>50</v>
@@ -3180,26 +3171,26 @@
         <v>42</v>
       </c>
       <c r="AJ19" t="s" s="2">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="AK19" t="s" s="2">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="AL19" t="s" s="2">
-        <v>177</v>
+        <v>183</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
-        <v>179</v>
+        <v>42</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" t="s" s="2">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="F20" t="s" s="2">
         <v>50</v>
@@ -3211,16 +3202,16 @@
         <v>42</v>
       </c>
       <c r="I20" t="s" s="2">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="J20" t="s" s="2">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
@@ -3271,10 +3262,10 @@
         <v>42</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="AF20" t="s" s="2">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="AG20" t="s" s="2">
         <v>50</v>
@@ -3286,18 +3277,18 @@
         <v>42</v>
       </c>
       <c r="AJ20" t="s" s="2">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="AK20" t="s" s="2">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="AL20" t="s" s="2">
-        <v>185</v>
+        <v>42</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
@@ -3311,7 +3302,7 @@
         <v>50</v>
       </c>
       <c r="G21" t="s" s="2">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="H21" t="s" s="2">
         <v>42</v>
@@ -3320,13 +3311,13 @@
         <v>42</v>
       </c>
       <c r="J21" t="s" s="2">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
@@ -3377,7 +3368,7 @@
         <v>42</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="AF21" t="s" s="2">
         <v>40</v>
@@ -3392,22 +3383,22 @@
         <v>42</v>
       </c>
       <c r="AJ21" t="s" s="2">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="AK21" t="s" s="2">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="AL21" t="s" s="2">
-        <v>42</v>
+        <v>196</v>
       </c>
     </row>
-    <row r="22" hidden="true">
+    <row r="22">
       <c r="A22" t="s" s="2">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
-        <v>42</v>
+        <v>198</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" t="s" s="2">
@@ -3417,7 +3408,7 @@
         <v>50</v>
       </c>
       <c r="G22" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="H22" t="s" s="2">
         <v>42</v>
@@ -3426,13 +3417,13 @@
         <v>42</v>
       </c>
       <c r="J22" t="s" s="2">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
@@ -3483,7 +3474,7 @@
         <v>42</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="AF22" t="s" s="2">
         <v>40</v>
@@ -3498,22 +3489,22 @@
         <v>42</v>
       </c>
       <c r="AJ22" t="s" s="2">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="AK22" t="s" s="2">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="AL22" t="s" s="2">
-        <v>198</v>
+        <v>42</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" t="s" s="2">
@@ -3523,24 +3514,26 @@
         <v>50</v>
       </c>
       <c r="G23" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="H23" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="I23" t="s" s="2">
         <v>51</v>
       </c>
-      <c r="H23" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="I23" t="s" s="2">
-        <v>42</v>
-      </c>
       <c r="J23" t="s" s="2">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>203</v>
-      </c>
-      <c r="M23" s="2"/>
+        <v>208</v>
+      </c>
+      <c r="M23" t="s" s="2">
+        <v>209</v>
+      </c>
       <c r="N23" s="2"/>
       <c r="O23" t="s" s="2">
         <v>42</v>
@@ -3589,7 +3582,7 @@
         <v>42</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>40</v>
@@ -3604,22 +3597,22 @@
         <v>42</v>
       </c>
       <c r="AJ23" t="s" s="2">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="AK23" t="s" s="2">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="AL23" t="s" s="2">
-        <v>42</v>
+        <v>212</v>
       </c>
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
-        <v>207</v>
+        <v>42</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" t="s" s="2">
@@ -3635,19 +3628,19 @@
         <v>42</v>
       </c>
       <c r="I24" t="s" s="2">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="J24" t="s" s="2">
-        <v>208</v>
+        <v>191</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="M24" t="s" s="2">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="N24" s="2"/>
       <c r="O24" t="s" s="2">
@@ -3697,7 +3690,7 @@
         <v>42</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>40</v>
@@ -3712,18 +3705,18 @@
         <v>42</v>
       </c>
       <c r="AJ24" t="s" s="2">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="AK24" t="s" s="2">
-        <v>213</v>
+        <v>42</v>
       </c>
       <c r="AL24" t="s" s="2">
-        <v>214</v>
+        <v>42</v>
       </c>
     </row>
-    <row r="25" hidden="true">
+    <row r="25">
       <c r="A25" t="s" s="2">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
@@ -3734,10 +3727,10 @@
         <v>40</v>
       </c>
       <c r="F25" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="G25" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="H25" t="s" s="2">
         <v>42</v>
@@ -3746,16 +3739,16 @@
         <v>42</v>
       </c>
       <c r="J25" t="s" s="2">
-        <v>193</v>
+        <v>219</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="M25" t="s" s="2">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="N25" s="2"/>
       <c r="O25" t="s" s="2">
@@ -3805,13 +3798,13 @@
         <v>42</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG25" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="AH25" t="s" s="2">
         <v>42</v>
@@ -3820,7 +3813,7 @@
         <v>42</v>
       </c>
       <c r="AJ25" t="s" s="2">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="AK25" t="s" s="2">
         <v>42</v>
@@ -3831,7 +3824,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s" s="2">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
@@ -3854,17 +3847,15 @@
         <v>42</v>
       </c>
       <c r="J26" t="s" s="2">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>223</v>
-      </c>
-      <c r="M26" t="s" s="2">
-        <v>224</v>
-      </c>
+        <v>227</v>
+      </c>
+      <c r="M26" s="2"/>
       <c r="N26" s="2"/>
       <c r="O26" t="s" s="2">
         <v>42</v>
@@ -3913,7 +3904,7 @@
         <v>42</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="AF26" t="s" s="2">
         <v>40</v>
@@ -3925,10 +3916,10 @@
         <v>42</v>
       </c>
       <c r="AI26" t="s" s="2">
-        <v>42</v>
+        <v>228</v>
       </c>
       <c r="AJ26" t="s" s="2">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="AK26" t="s" s="2">
         <v>42</v>
@@ -3937,9 +3928,9 @@
         <v>42</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
@@ -3950,10 +3941,10 @@
         <v>40</v>
       </c>
       <c r="F27" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="G27" t="s" s="2">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="H27" t="s" s="2">
         <v>42</v>
@@ -3962,13 +3953,13 @@
         <v>42</v>
       </c>
       <c r="J27" t="s" s="2">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
@@ -4019,22 +4010,22 @@
         <v>42</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>226</v>
+        <v>234</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG27" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="AH27" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AI27" t="s" s="2">
-        <v>230</v>
+        <v>42</v>
       </c>
       <c r="AJ27" t="s" s="2">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="AK27" t="s" s="2">
         <v>42</v>
@@ -4045,18 +4036,18 @@
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
-        <v>42</v>
+        <v>108</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" t="s" s="2">
         <v>40</v>
       </c>
       <c r="F28" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="G28" t="s" s="2">
         <v>42</v>
@@ -4068,15 +4059,17 @@
         <v>42</v>
       </c>
       <c r="J28" t="s" s="2">
-        <v>233</v>
+        <v>95</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>235</v>
-      </c>
-      <c r="M28" s="2"/>
+        <v>238</v>
+      </c>
+      <c r="M28" t="s" s="2">
+        <v>111</v>
+      </c>
       <c r="N28" s="2"/>
       <c r="O28" t="s" s="2">
         <v>42</v>
@@ -4125,13 +4118,13 @@
         <v>42</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG28" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="AH28" t="s" s="2">
         <v>42</v>
@@ -4140,7 +4133,7 @@
         <v>42</v>
       </c>
       <c r="AJ28" t="s" s="2">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="AK28" t="s" s="2">
         <v>42</v>
@@ -4151,11 +4144,11 @@
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
-        <v>110</v>
+        <v>241</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" t="s" s="2">
@@ -4168,22 +4161,22 @@
         <v>42</v>
       </c>
       <c r="H29" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="I29" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="J29" t="s" s="2">
         <v>95</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>239</v>
+        <v>109</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="N29" s="2"/>
       <c r="O29" t="s" s="2">
@@ -4233,7 +4226,7 @@
         <v>42</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>40</v>
@@ -4248,7 +4241,7 @@
         <v>42</v>
       </c>
       <c r="AJ29" t="s" s="2">
-        <v>237</v>
+        <v>93</v>
       </c>
       <c r="AK29" t="s" s="2">
         <v>42</v>
@@ -4257,41 +4250,41 @@
         <v>42</v>
       </c>
     </row>
-    <row r="30" hidden="true">
+    <row r="30">
       <c r="A30" t="s" s="2">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
-        <v>243</v>
+        <v>42</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" t="s" s="2">
         <v>40</v>
       </c>
       <c r="F30" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="G30" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="H30" t="s" s="2">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="I30" t="s" s="2">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="J30" t="s" s="2">
-        <v>95</v>
+        <v>166</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>111</v>
+        <v>245</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>113</v>
+        <v>247</v>
       </c>
       <c r="N30" s="2"/>
       <c r="O30" t="s" s="2">
@@ -4317,13 +4310,13 @@
         <v>42</v>
       </c>
       <c r="W30" t="s" s="2">
-        <v>42</v>
+        <v>170</v>
       </c>
       <c r="X30" t="s" s="2">
-        <v>42</v>
+        <v>248</v>
       </c>
       <c r="Y30" t="s" s="2">
-        <v>42</v>
+        <v>249</v>
       </c>
       <c r="Z30" t="s" s="2">
         <v>42</v>
@@ -4341,13 +4334,13 @@
         <v>42</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG30" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="AH30" t="s" s="2">
         <v>42</v>
@@ -4356,7 +4349,7 @@
         <v>42</v>
       </c>
       <c r="AJ30" t="s" s="2">
-        <v>93</v>
+        <v>250</v>
       </c>
       <c r="AK30" t="s" s="2">
         <v>42</v>
@@ -4367,18 +4360,18 @@
     </row>
     <row r="31">
       <c r="A31" t="s" s="2">
-        <v>246</v>
+        <v>251</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
-        <v>42</v>
+        <v>252</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="F31" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="G31" t="s" s="2">
         <v>51</v>
@@ -4390,16 +4383,16 @@
         <v>42</v>
       </c>
       <c r="J31" t="s" s="2">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="N31" s="2"/>
       <c r="O31" t="s" s="2">
@@ -4425,37 +4418,37 @@
         <v>42</v>
       </c>
       <c r="W31" t="s" s="2">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="X31" t="s" s="2">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="Y31" t="s" s="2">
+        <v>257</v>
+      </c>
+      <c r="Z31" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AA31" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AB31" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AC31" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AD31" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AE31" t="s" s="2">
         <v>251</v>
       </c>
-      <c r="Z31" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AA31" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AB31" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AC31" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AD31" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AE31" t="s" s="2">
-        <v>246</v>
-      </c>
       <c r="AF31" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="AG31" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="AH31" t="s" s="2">
         <v>42</v>
@@ -4464,32 +4457,32 @@
         <v>42</v>
       </c>
       <c r="AJ31" t="s" s="2">
-        <v>252</v>
+        <v>142</v>
       </c>
       <c r="AK31" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AL31" t="s" s="2">
-        <v>42</v>
+        <v>258</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>253</v>
+        <v>259</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" t="s" s="2">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="F32" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="G32" t="s" s="2">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="H32" t="s" s="2">
         <v>42</v>
@@ -4498,16 +4491,16 @@
         <v>42</v>
       </c>
       <c r="J32" t="s" s="2">
-        <v>168</v>
+        <v>231</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>255</v>
+        <v>261</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>256</v>
+        <v>262</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>257</v>
+        <v>263</v>
       </c>
       <c r="N32" s="2"/>
       <c r="O32" t="s" s="2">
@@ -4533,37 +4526,37 @@
         <v>42</v>
       </c>
       <c r="W32" t="s" s="2">
-        <v>172</v>
+        <v>42</v>
       </c>
       <c r="X32" t="s" s="2">
-        <v>258</v>
+        <v>42</v>
       </c>
       <c r="Y32" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="Z32" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AA32" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AB32" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AC32" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AD32" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AE32" t="s" s="2">
         <v>259</v>
       </c>
-      <c r="Z32" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AA32" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AB32" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AC32" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AD32" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AE32" t="s" s="2">
-        <v>253</v>
-      </c>
       <c r="AF32" t="s" s="2">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="AG32" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="AH32" t="s" s="2">
         <v>42</v>
@@ -4572,22 +4565,22 @@
         <v>42</v>
       </c>
       <c r="AJ32" t="s" s="2">
-        <v>144</v>
+        <v>264</v>
       </c>
       <c r="AK32" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AL32" t="s" s="2">
-        <v>260</v>
+        <v>42</v>
       </c>
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
-        <v>262</v>
+        <v>42</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" t="s" s="2">
@@ -4606,17 +4599,15 @@
         <v>42</v>
       </c>
       <c r="J33" t="s" s="2">
-        <v>233</v>
+        <v>191</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>264</v>
-      </c>
-      <c r="M33" t="s" s="2">
-        <v>265</v>
-      </c>
+        <v>267</v>
+      </c>
+      <c r="M33" s="2"/>
       <c r="N33" s="2"/>
       <c r="O33" t="s" s="2">
         <v>42</v>
@@ -4665,7 +4656,7 @@
         <v>42</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>40</v>
@@ -4680,18 +4671,18 @@
         <v>42</v>
       </c>
       <c r="AJ33" t="s" s="2">
-        <v>266</v>
+        <v>188</v>
       </c>
       <c r="AK33" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AL33" t="s" s="2">
-        <v>42</v>
+        <v>268</v>
       </c>
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
@@ -4714,15 +4705,17 @@
         <v>42</v>
       </c>
       <c r="J34" t="s" s="2">
-        <v>193</v>
+        <v>69</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>269</v>
-      </c>
-      <c r="M34" s="2"/>
+        <v>271</v>
+      </c>
+      <c r="M34" t="s" s="2">
+        <v>272</v>
+      </c>
       <c r="N34" s="2"/>
       <c r="O34" t="s" s="2">
         <v>42</v>
@@ -4747,13 +4740,13 @@
         <v>42</v>
       </c>
       <c r="W34" t="s" s="2">
-        <v>42</v>
+        <v>123</v>
       </c>
       <c r="X34" t="s" s="2">
-        <v>42</v>
+        <v>273</v>
       </c>
       <c r="Y34" t="s" s="2">
-        <v>42</v>
+        <v>274</v>
       </c>
       <c r="Z34" t="s" s="2">
         <v>42</v>
@@ -4771,7 +4764,7 @@
         <v>42</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>40</v>
@@ -4786,18 +4779,18 @@
         <v>42</v>
       </c>
       <c r="AJ34" t="s" s="2">
-        <v>190</v>
+        <v>161</v>
       </c>
       <c r="AK34" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AL34" t="s" s="2">
-        <v>270</v>
+        <v>42</v>
       </c>
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -4820,16 +4813,16 @@
         <v>42</v>
       </c>
       <c r="J35" t="s" s="2">
-        <v>69</v>
+        <v>166</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="M35" t="s" s="2">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="N35" s="2"/>
       <c r="O35" t="s" s="2">
@@ -4855,32 +4848,32 @@
         <v>42</v>
       </c>
       <c r="W35" t="s" s="2">
-        <v>125</v>
+        <v>279</v>
       </c>
       <c r="X35" t="s" s="2">
+        <v>280</v>
+      </c>
+      <c r="Y35" t="s" s="2">
+        <v>281</v>
+      </c>
+      <c r="Z35" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AA35" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AB35" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AC35" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AD35" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AE35" t="s" s="2">
         <v>275</v>
       </c>
-      <c r="Y35" t="s" s="2">
-        <v>276</v>
-      </c>
-      <c r="Z35" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AA35" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AB35" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AC35" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AD35" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AE35" t="s" s="2">
-        <v>271</v>
-      </c>
       <c r="AF35" t="s" s="2">
         <v>40</v>
       </c>
@@ -4894,7 +4887,7 @@
         <v>42</v>
       </c>
       <c r="AJ35" t="s" s="2">
-        <v>163</v>
+        <v>282</v>
       </c>
       <c r="AK35" t="s" s="2">
         <v>42</v>
@@ -4905,7 +4898,7 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -4916,7 +4909,7 @@
         <v>40</v>
       </c>
       <c r="F36" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="G36" t="s" s="2">
         <v>42</v>
@@ -4928,16 +4921,16 @@
         <v>42</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>168</v>
+        <v>219</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>278</v>
+        <v>284</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="M36" t="s" s="2">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="N36" s="2"/>
       <c r="O36" t="s" s="2">
@@ -4963,37 +4956,37 @@
         <v>42</v>
       </c>
       <c r="W36" t="s" s="2">
-        <v>281</v>
+        <v>42</v>
       </c>
       <c r="X36" t="s" s="2">
-        <v>282</v>
+        <v>42</v>
       </c>
       <c r="Y36" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="Z36" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AA36" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AB36" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AC36" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AD36" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AE36" t="s" s="2">
         <v>283</v>
       </c>
-      <c r="Z36" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AA36" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AB36" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AC36" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AD36" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AE36" t="s" s="2">
-        <v>277</v>
-      </c>
       <c r="AF36" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG36" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="AH36" t="s" s="2">
         <v>42</v>
@@ -5002,125 +4995,17 @@
         <v>42</v>
       </c>
       <c r="AJ36" t="s" s="2">
-        <v>284</v>
+        <v>223</v>
       </c>
       <c r="AK36" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AL36" t="s" s="2">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="37" hidden="true">
-      <c r="A37" t="s" s="2">
-        <v>285</v>
-      </c>
-      <c r="B37" s="2"/>
-      <c r="C37" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="D37" s="2"/>
-      <c r="E37" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="F37" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="G37" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="H37" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="I37" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="J37" t="s" s="2">
-        <v>221</v>
-      </c>
-      <c r="K37" t="s" s="2">
-        <v>286</v>
-      </c>
-      <c r="L37" t="s" s="2">
-        <v>287</v>
-      </c>
-      <c r="M37" t="s" s="2">
-        <v>288</v>
-      </c>
-      <c r="N37" s="2"/>
-      <c r="O37" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="P37" s="2"/>
-      <c r="Q37" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="R37" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="S37" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="T37" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="U37" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="V37" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="W37" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="X37" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="Y37" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="Z37" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AA37" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AB37" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AC37" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AD37" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AE37" t="s" s="2">
-        <v>285</v>
-      </c>
-      <c r="AF37" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AG37" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AH37" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AI37" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AJ37" t="s" s="2">
-        <v>225</v>
-      </c>
-      <c r="AK37" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AL37" t="s" s="2">
         <v>42</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AL37">
+  <autoFilter ref="A1:AL36">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -5130,7 +5015,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI36">
+  <conditionalFormatting sqref="A2:AI35">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>